<commit_message>
Mass imports with Excel: read (start) and adapt to new table format
</commit_message>
<xml_diff>
--- a/shanoir-uploader/src/test/resources/template_pacs_import.xlsx
+++ b/shanoir-uploader/src/test/resources/template_pacs_import.xlsx
@@ -20,38 +20,35 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="21">
   <si>
     <t xml:space="preserve">DICOM_QUERY_LEVEL</t>
   </si>
   <si>
+    <t xml:space="preserve">DICOM_PATIENT_NAME</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DICOM_PATIENT_ID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DICOM_PATIENT_BIRTH_DATE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DICOM_STUDY_DESCRIPTION</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DICOM_STUDY_DATE</t>
+  </si>
+  <si>
     <t xml:space="preserve">DICOM_MODALITY</t>
   </si>
   <si>
-    <t xml:space="preserve">DICOM_PATIENT_FAMILY_NAME</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DICOM_PATIENT_GIVEN_NAME</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DICOM_PATIENT_BIRTH_NAME</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DICOM_PATIENT_BIRTH_DATE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DICOM_STUDY_DATE</t>
+    <t xml:space="preserve">DICOM_STUDY_DESCRIPTION_FILTER</t>
   </si>
   <si>
     <t xml:space="preserve">DICOM_STUDY_DATE_FILTER</t>
   </si>
   <si>
-    <t xml:space="preserve">DICOM_STUDY_DESCRIPTION</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DICOM_STUDY_DESCRIPTION_FILTER</t>
-  </si>
-  <si>
     <t xml:space="preserve">DICOM_SERIES_FILTER</t>
   </si>
   <si>
@@ -67,7 +64,10 @@
     <t xml:space="preserve">SHANOIR_EXAM_COMMENT</t>
   </si>
   <si>
-    <t xml:space="preserve">S</t>
+    <t xml:space="preserve">STUDY</t>
+  </si>
+  <si>
+    <t xml:space="preserve">keiler</t>
   </si>
   <si>
     <t xml:space="preserve">MR</t>
@@ -80,21 +80,26 @@
   </si>
   <si>
     <t xml:space="preserve">if empty use from dicom</t>
+  </si>
+  <si>
+    <t xml:space="preserve">New_Peter_Pan</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd"/>
+    <numFmt numFmtId="165" formatCode="@"/>
+    <numFmt numFmtId="166" formatCode="yyyy\-mm\-dd"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -111,13 +116,38 @@
       <name val="Arial"/>
       <family val="0"/>
     </font>
+    <font>
+      <b val="true"/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCCCCCC"/>
+        <bgColor rgb="FFCCCCFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF729FCF"/>
+        <bgColor rgb="FF969696"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF800080"/>
+        <bgColor rgb="FF800080"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -154,12 +184,32 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="7">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -172,6 +222,66 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
     <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008000"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FF808000"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FFCCCCCC"/>
+      <rgbColor rgb="FF808080"/>
+      <rgbColor rgb="FF729FCF"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FFFFFFCC"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FF660066"/>
+      <rgbColor rgb="FFFF8080"/>
+      <rgbColor rgb="FF0066CC"/>
+      <rgbColor rgb="FFCCCCFF"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FF00CCFF"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FFCCFFCC"/>
+      <rgbColor rgb="FFFFFF99"/>
+      <rgbColor rgb="FF99CCFF"/>
+      <rgbColor rgb="FFFF99CC"/>
+      <rgbColor rgb="FFCC99FF"/>
+      <rgbColor rgb="FFFFCC99"/>
+      <rgbColor rgb="FF3366FF"/>
+      <rgbColor rgb="FF33CCCC"/>
+      <rgbColor rgb="FF99CC00"/>
+      <rgbColor rgb="FFFFCC00"/>
+      <rgbColor rgb="FFFF9900"/>
+      <rgbColor rgb="FFFF6600"/>
+      <rgbColor rgb="FF666699"/>
+      <rgbColor rgb="FF969696"/>
+      <rgbColor rgb="FF003366"/>
+      <rgbColor rgb="FF339966"/>
+      <rgbColor rgb="FF003300"/>
+      <rgbColor rgb="FF333300"/>
+      <rgbColor rgb="FF993300"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FF333399"/>
+      <rgbColor rgb="FF333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -286,110 +396,118 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:O4"/>
+  <dimension ref="A1:N4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E2" activeCellId="0" sqref="E2"/>
+      <selection pane="topLeft" activeCell="G1" activeCellId="0" sqref="A:G"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="21.59"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="17.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="30.23"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="29.25"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="28.97"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="28.55"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="20.49"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="27.72"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="35.24"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="22.58"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="19.65"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="34.96"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="22.3"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="21.18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="21.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="22.58"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="20.35"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="28.55"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="20.49"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="17.98"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="2" width="35.37"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="2" width="27.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="2" width="22.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="2" width="19.65"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="2" width="34.97"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="2" width="25.35"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="2" width="26.32"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="0" t="s">
+      <c r="E1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="0" t="s">
+      <c r="F1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="0" t="s">
+      <c r="G1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="0" t="s">
+      <c r="H1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="0" t="s">
+      <c r="I1" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="0" t="s">
+      <c r="J1" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="0" t="s">
+      <c r="K1" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="0" t="s">
+      <c r="L1" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="0" t="s">
+      <c r="M1" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="0" t="s">
+      <c r="N1" s="5" t="s">
         <v>13</v>
-      </c>
-      <c r="O1" s="0" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="A2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="F2" s="1" t="n">
+        <v>20100304</v>
+      </c>
+      <c r="G2" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="H2" s="1" t="n">
-        <v>42736</v>
-      </c>
-      <c r="L2" s="0" t="n">
+      <c r="I2" s="6"/>
+      <c r="K2" s="2" t="n">
         <v>17</v>
       </c>
-      <c r="M2" s="0" t="s">
+      <c r="L2" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="N2" s="0" t="s">
+      <c r="M2" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="O2" s="0" t="s">
+      <c r="N2" s="2" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H3" s="1" t="n">
-        <v>42736</v>
-      </c>
+      <c r="A3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F3" s="1" t="n">
+        <v>20180424</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I3" s="6"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H4" s="1" t="n">
-        <v>42736</v>
-      </c>
+      <c r="I4" s="6"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
Excel import: some fixes, now download from pacs works
</commit_message>
<xml_diff>
--- a/shanoir-uploader/src/test/resources/template_pacs_import.xlsx
+++ b/shanoir-uploader/src/test/resources/template_pacs_import.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="22">
   <si>
     <t xml:space="preserve">DICOM_QUERY_LEVEL</t>
   </si>
@@ -43,16 +43,49 @@
     <t xml:space="preserve">DICOM_MODALITY</t>
   </si>
   <si>
-    <t xml:space="preserve">DICOM_STUDY_DESCRIPTION_FILTER</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DICOM_STUDY_DATE_FILTER</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DICOM_SERIES_FILTER</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SHANOIR_STUDY_ID</t>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">FILTER_</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">DICOM_STUDY_DESCRIPTION</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">FILTER_</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">DICOM_STUDY_MIN_DATE</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">FILTER_DICOM_SERIES_DESCRIPTION</t>
   </si>
   <si>
     <t xml:space="preserve">SHANOIR_STUDY_CARD_NAME</t>
@@ -70,7 +103,7 @@
     <t xml:space="preserve">keiler</t>
   </si>
   <si>
-    <t xml:space="preserve">20100403</t>
+    <t xml:space="preserve">20100304</t>
   </si>
   <si>
     <t xml:space="preserve">MR</t>
@@ -100,7 +133,7 @@
     <numFmt numFmtId="165" formatCode="@"/>
     <numFmt numFmtId="166" formatCode="yyyy\-mm\-dd"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -128,6 +161,12 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="5">
@@ -190,7 +229,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -204,6 +243,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -402,10 +445,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:N3"/>
+  <dimension ref="A1:M3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J2" activeCellId="0" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -418,12 +461,11 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="20.49"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="17.98"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="2" width="35.37"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="2" width="27.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="2" width="22.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="2" width="19.65"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="2" width="34.97"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="2" width="25.35"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="2" width="26.32"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="2" width="33.38"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="2" width="36.06"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="2" width="34.97"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="2" width="25.35"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="2" width="26.32"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -454,37 +496,34 @@
       <c r="I1" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="J1" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="5" t="s">
+      <c r="K1" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="5" t="s">
+      <c r="L1" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="5" t="s">
+      <c r="M1" s="6" t="s">
         <v>12</v>
-      </c>
-      <c r="N1" s="5" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="F2" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="G2" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="G2" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="I2" s="6"/>
-      <c r="K2" s="2" t="n">
+      <c r="I2" s="7"/>
+      <c r="K2" s="2" t="s">
         <v>17</v>
       </c>
       <c r="L2" s="2" t="s">
@@ -492,25 +531,22 @@
       </c>
       <c r="M2" s="2" t="s">
         <v>19</v>
-      </c>
-      <c r="N2" s="2" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F3" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="F3" s="1" t="s">
-        <v>22</v>
-      </c>
       <c r="G3" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="I3" s="6"/>
+        <v>16</v>
+      </c>
+      <c r="I3" s="7"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
Move DatasetModalityType to ms-common and now create manu + manuModel in mass import
</commit_message>
<xml_diff>
--- a/shanoir-uploader/src/test/resources/template_pacs_import.xlsx
+++ b/shanoir-uploader/src/test/resources/template_pacs_import.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="21">
   <si>
     <t xml:space="preserve">DICOM_QUERY_LEVEL</t>
   </si>
@@ -76,22 +76,13 @@
     <t xml:space="preserve">STUDY</t>
   </si>
   <si>
-    <t xml:space="preserve">keiler</t>
-  </si>
-  <si>
     <t xml:space="preserve">20100304</t>
   </si>
   <si>
     <t xml:space="preserve">MR</t>
   </si>
   <si>
-    <t xml:space="preserve">Keiler-exam</t>
-  </si>
-  <si>
-    <t xml:space="preserve">New_Peter_Pan</t>
-  </si>
-  <si>
-    <t xml:space="preserve">20180424</t>
+    <t xml:space="preserve">01/01/2018</t>
   </si>
 </sst>
 </file>
@@ -103,7 +94,7 @@
     <numFmt numFmtId="165" formatCode="@"/>
     <numFmt numFmtId="166" formatCode="yyyy\-mm\-dd"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -131,12 +122,6 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="6">
@@ -230,7 +215,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="165" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -427,8 +412,8 @@
   </sheetPr>
   <dimension ref="A1:Q3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L12" activeCellId="0" sqref="L12"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="H1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="K3" activeCellId="0" sqref="K3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -443,7 +428,9 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="2" width="35.37"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="2" width="33.38"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="2" width="36.06"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="11" style="2" width="34.97"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="11" style="2" width="34.97"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="34.97"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="2" width="34.97"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="2" width="25.35"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="2" width="26.32"/>
   </cols>
@@ -485,7 +472,7 @@
       <c r="L1" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="6" t="s">
+      <c r="M1" s="5" t="s">
         <v>12</v>
       </c>
       <c r="N1" s="6" t="s">
@@ -505,37 +492,31 @@
       <c r="A2" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="F2" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="G2" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="I2" s="8"/>
+      <c r="N2" s="1" t="s">
         <v>20</v>
-      </c>
-      <c r="I2" s="8"/>
-      <c r="P2" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="Q2" s="2" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>22</v>
-      </c>
       <c r="F3" s="1" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="G3" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="I3" s="8"/>
+      <c r="N3" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="I3" s="8"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>